<commit_message>
Added Silica Gel to BOM (It's kind of important!) and price for PCB.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="119">
   <si>
     <t>Acrylic Sheet</t>
   </si>
@@ -366,6 +366,21 @@
   </si>
   <si>
     <t>http://www.ebay.co.uk/itm/like/291536178882</t>
+  </si>
+  <si>
+    <t>Silica Gel</t>
+  </si>
+  <si>
+    <t>1kg</t>
+  </si>
+  <si>
+    <t>http://www.ebay.co.uk/itm/1000g-1kg-BONUS-100g-BAG-Silica-Gel-Desiccant-Self-Indicating-Loose-/111737656127?hash=item1a0415533f:g:340AAOSwu4BVm9lH</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>USD 20 - for 3.</t>
   </si>
 </sst>
 </file>
@@ -707,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K38"/>
+  <dimension ref="A2:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H38"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,131 +943,137 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12">
+        <v>8.9499999999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14">
-        <v>10.43</v>
-      </c>
-      <c r="K14" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15">
+        <v>10.43</v>
+      </c>
+      <c r="K15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" t="s">
-        <v>95</v>
+        <v>29</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="H19">
-        <v>19.98</v>
-      </c>
-      <c r="I19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" t="s">
-        <v>96</v>
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>107</v>
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>95</v>
       </c>
       <c r="H20">
-        <v>1.69</v>
-      </c>
-      <c r="K20" t="s">
-        <v>108</v>
+        <v>19.98</v>
+      </c>
+      <c r="I20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1856422</v>
+        <v>54</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="H21">
-        <v>0.04</v>
+        <v>1.69</v>
+      </c>
+      <c r="K21" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1060,91 +1081,91 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F22" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>97</v>
+      <c r="G22" s="1">
+        <v>1856422</v>
       </c>
       <c r="H22">
-        <v>6.6000000000000003E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F23" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23">
+        <v>6.6000000000000003E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24">
-        <v>7805</v>
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H24">
-        <v>1.83</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="C25">
+        <v>7805</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="1">
-        <v>9731148</v>
+        <v>54</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="H25">
-        <v>8.4000000000000005E-2</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
         <v>64</v>
@@ -1159,18 +1180,21 @@
         <v>66</v>
       </c>
       <c r="G26" s="1">
-        <v>143126</v>
+        <v>9731148</v>
       </c>
       <c r="H26">
-        <v>0.13500000000000001</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>65</v>
@@ -1178,46 +1202,48 @@
       <c r="F27" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="2">
-        <v>2424111</v>
+      <c r="G27" s="1">
+        <v>143126</v>
       </c>
       <c r="H27">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="K27" t="s">
-        <v>101</v>
+        <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F28" t="s">
         <v>66</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="2">
+        <v>2424111</v>
+      </c>
+      <c r="H28">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="K28" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F29" t="s">
         <v>66</v>
@@ -1226,194 +1252,222 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F30" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="1">
-        <v>1081225</v>
-      </c>
-      <c r="H30">
-        <v>0.03</v>
-      </c>
+      <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F31" t="s">
         <v>66</v>
       </c>
       <c r="G31" s="1">
-        <v>1894738</v>
+        <v>1081225</v>
       </c>
       <c r="H31">
-        <v>0.14000000000000001</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F32" t="s">
         <v>66</v>
       </c>
       <c r="G32" s="1">
-        <v>9731156</v>
+        <v>1894738</v>
       </c>
       <c r="H32">
-        <v>0.17399999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>85</v>
-      </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1">
+        <v>9731156</v>
+      </c>
+      <c r="H33">
+        <v>0.17399999999999999</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="E34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F34" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="1">
-        <v>1081225</v>
-      </c>
-      <c r="H34">
-        <v>0.03</v>
-      </c>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F35" t="s">
         <v>66</v>
       </c>
+      <c r="G35" s="1">
+        <v>1081225</v>
+      </c>
+      <c r="H35">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
+      <c r="E36" t="s">
+        <v>90</v>
+      </c>
       <c r="F36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H36">
-        <v>1.5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
       </c>
       <c r="D37">
-        <v>4</v>
-      </c>
-      <c r="K37" t="s">
-        <v>93</v>
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37">
+        <v>1.5</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="K38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>104</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>103</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
         <v>54</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H38">
+      <c r="H39">
         <v>2.4900000000000002</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K39" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>117</v>
+      </c>
+      <c r="H45">
+        <f>SUM(H4:H44)</f>
+        <v>108.58300000000001</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G36" r:id="rId1"/>
-    <hyperlink ref="G38" r:id="rId2"/>
+    <hyperlink ref="G37" r:id="rId1"/>
+    <hyperlink ref="G39" r:id="rId2"/>
+    <hyperlink ref="G19" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>